<commit_message>
:sparkles: 기본 데이터 베이스 ScriptableObject와 연동
</commit_message>
<xml_diff>
--- a/Assets/Resources/GameData/BarGuestDB.xlsx
+++ b/Assets/Resources/GameData/BarGuestDB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\UnityMyGame\Nemesis1842\Assets\Resources\GameData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC14B09A-42B7-4594-857C-2955CE06E8CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA4C35CD-266E-47F6-A669-0C00FC44FD52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{5617D017-30E4-41E9-B447-248D8C09DB73}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5617D017-30E4-41E9-B447-248D8C09DB73}"/>
   </bookViews>
   <sheets>
     <sheet name="Guests" sheetId="2" r:id="rId1"/>
@@ -596,7 +596,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="43">
   <si>
     <t>guest_code</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -606,10 +606,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>아니야</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>day</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -622,62 +618,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>꺼져</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>수강신청 제발</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>주원아 술 좀 그만 마셔라</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>지혁아 작업 좀 빨리 빨리 하자</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>알았지 ^^</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>character_name</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>베일 존</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>임주원</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>술이 최고야</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>술 너가 유일한 친구야</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>소주 vs 양주?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>다음에는 다이키리 먹어야지 허허</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>아 2차는 어디로 갈까</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>밴드부에서 마셔야징</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>character_code</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -734,7 +678,94 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>아니요</t>
+    <t>미아</t>
+  </si>
+  <si>
+    <t>미아</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>여긴 본 적이 없는데 최근에 개업하셨나봐요?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이런 시골 촌에도 입주를 하는 사람이 있구나~</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>나는 상큼하고 신 걸 좋아해요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>뭐 칵테일을 먹어본 적은 없지만..</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>뭐 주문 내용은 이해하셨겠죠?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>내가 칵테일에 대해 아는 건 없지만..</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>옆 집 펍보다는 그나마 나은 수준이네요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>뭐 현실적으로 번창하라는 말은 못하겠지만.. 열심히 해보세요~</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>다니엘</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>여기가 친구가 말한 바가 맞겠지?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>새로 생긴 바가 있다고 해서 친구놈이 실험쥐로 날 먼저 보냈어</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이 동네 사람들은 바라는 곳을 한 번도 가본 적이 없어서 아마 시내에 한 번이라도 가본 나를 앞세운 거겠지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>뭐 나도 사실상 바를 한 번도 가본 적은 없지만 말이야 하..</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>하하..</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>너 생각보다 말이 없구나?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>됐어 그럼. 내가 지금 외롭기도 하고.. 우울감도 좀 있는 것 같아서 아무한테나 말을 걸고 싶었거든</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이렇게 주문하는게 맞나?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아무튼 바텐더, 오늘 내 기분대로 한 잔~</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>뭐 맥주만 마시던 내가 원하던 느낌은 아니지만..</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일단 취하니까 기분은 좋네~</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>번창하쇼~ 아니 번창은 힘들겠구나..</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1144,8 +1175,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5A3813C-C140-4D5B-9DC5-AEE517EEDFFA}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1160,18 +1191,18 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
       <c r="D1" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1180,12 +1211,12 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -1194,12 +1225,12 @@
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1208,7 +1239,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1219,10 +1250,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{587ECBB5-A40B-459B-A765-E9FD0D7D4D73}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1230,7 +1261,7 @@
     <col min="1" max="1" width="12.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.375" customWidth="1"/>
     <col min="3" max="3" width="20.625" customWidth="1"/>
-    <col min="4" max="4" width="67.75" customWidth="1"/>
+    <col min="4" max="4" width="90.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -1238,10 +1269,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
         <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>11</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -1249,170 +1280,282 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
         <v>21</v>
       </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D9" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="D10" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="D11" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="D12" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19">
         <v>1</v>
       </c>
-      <c r="C13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" t="s">
-        <v>19</v>
+      <c r="C19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1424,10 +1567,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4ED8E90-E9EF-4636-A305-9B13E1C654FB}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1443,27 +1586,27 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D1" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="E1" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -1474,52 +1617,35 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
:memo: bar 내부/외부 script
바 내 외부 대사
</commit_message>
<xml_diff>
--- a/Assets/Resources/GameData/BarGuestDB.xlsx
+++ b/Assets/Resources/GameData/BarGuestDB.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\UnityMyGame\Nemesis1842\Assets\Resources\GameData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\test\Nemesis1842\Assets\Resources\GameData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6227D3E1-80E8-4BA4-805C-BB3BE32B5523}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6E29ADD-6710-46AB-8AED-826FE7AD1479}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{5617D017-30E4-41E9-B447-248D8C09DB73}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21840" activeTab="4" xr2:uid="{5617D017-30E4-41E9-B447-248D8C09DB73}"/>
   </bookViews>
   <sheets>
     <sheet name="Guests" sheetId="2" r:id="rId1"/>
@@ -129,7 +129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="90">
   <si>
     <t>guest_code</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -223,74 +223,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>끄아 취한다~</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(기절)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>엄마가 보고싶은 칵테일을 달라고 한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">바가 너무 허름하군 </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>오랜만이네~</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>그거 알아? 4일 전에 김주호가 생일이였데</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>김주호 생일은 10월 9일이니까 잘 기억해둬~</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>검정 검정한 칵테일로~</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>캬~ ㅣㅇ 거야~</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>더 마실 수 있겠는 걸?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>근데 그거 알아?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>좀 있으면 김지혁도 생일이래~</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>잘 기억하라고~?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>내심 기대하고 있을거니까 안해주면 삐질거야 아마..</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>엄마가 보고 싶은 칵테일로 한잔~</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ㅣ ㄱ ㅓㄴ야ㅑㅑㅏ~</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>WASTED</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>triangle_leaven_count</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -299,10 +231,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>올리언스 마을의 달 같은 칵테일로</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>셀레나</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -331,38 +259,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>올리언스 마을의 달 같은 칵테일 하나.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>달달한 설탕 맛이 나는 칵테일로.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>달이라고 달! Moon 몰라?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Moon이라고 너 영어 몇등급이야?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>분명 내가 달 같은 걸 달라고 했을텐데.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>그런 거 말고 설탕이 들어간 느낌이야.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>이거 말고 설탕 같은 재료를 넣어.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>설탕 Sugar!! 말귀를 왜 못 알아 먹는거야!</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>answer_alcohol</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -408,6 +304,189 @@
   </si>
   <si>
     <t>3일까지 잘 준비해보라고 크킄..</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>콜먼 오랜만이네 요즘 기분이 별로 안좋네.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>뭔가 입안이 화해 지면서 시원한 칵테일을 마시고 싶군.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>혹시 이런 비슷한 칵테일 한잔 주겠나?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이 기분이면 제일 독한걸로 한잔 더 가능하겠…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>홍홍…(기절)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>음! 콜먼 역시 당신 실력은 최고야 !</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>콜먼~요즘 바빠서 많이 못왔어요. 미안해요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>제 마음과 같은 칵테일 한잔 줘요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>오랜만에 콜먼을 보니 제 마음이 핑크빛 이네요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>콜먼…! 내가 당신 실력을 평생 가지고 싶어요. 어쩜 이리 잘만들까요..?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>한잔 더 줄래요?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">음.. 제가 내일 스케쥴이 있어서.. 더 많이 취하면 안될 것 같은데.. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그럼 얼음 처럼 시원해 보이는 칵테일 한잔 줘..클클…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(흠흠) 클클이라니… 저 원래 이렇게 안웃어요 흥.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">어쩜 이리 맛있는 칵테일을 계속 해서 만들어 줄 수있어? </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>당신은 천재인것 같아!!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>클클클클클..</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>으ㅡ음.. 제가 많이 취했나보 ㅏ…요..</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>읗흐흫ㅎ .. 킥킥ㅋ기 콜먼.. 당신은 내..가..ㄱ.ㅏ.질..꺼..야..</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>클클…(기절)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>으음…? 콜먼.. 당신 나랑 장난해요? 다시 줘요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>누가 보면 다른 사람이 만든줄 알겠어요. 다시주세요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>으윽.. 전혀 내 취향이 아니잖아!! 다시 내놔!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>흠…? 자네 오늘은 컨디션이 별로 인가 보군! 다시 내놓으시게!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>퉷 바다의 쓴맛보다 더 맛없다고!! 다시 줘!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>정말 아쉬운 맛이군요. 다시 부탁드려요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>끄윽 맛없어.. 다시 줘요..</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>퉤퉤퉤.. 제가 고급 입맛이라.. 제 취향 알잖아요? 다시 주세요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>우웩.. 이건 아니잖아요.. 오늘 솜씨가 엉망이네요. 다시 주세요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>핑크색 구름처럼 보이는 우아한 칵테일을 달라고 한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>얼음처럼 차가우며 은은한 달빛이 연상되는 칵테일을 달라고한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>민트 처럼 입안이 화해지며 은하수처럼 반짝 거리는 칵테일을 달라고 한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Two_hands_chin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Normal_stage_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Two_hands_table</t>
+  </si>
+  <si>
+    <t>Two_hands_table</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0004</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>어이 퇴근하는 거냐?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>돈은 꽤 벌었고? 어서 모아~키킼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0005</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>콜먼! 자네 퇴근하는건가?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>나도 한번 들어야하는데 요새 일이 너무 많군</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0006</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아깐 내가 꼬장 부려 미안하네!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아무튼 다음에도 잘 부탁하겠네!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>콜먼! 오늘 잘마셨다!</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -878,7 +957,7 @@
   <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -886,7 +965,7 @@
     <col min="1" max="1" width="11.125" customWidth="1"/>
     <col min="2" max="2" width="10.25" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="69.625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.25" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.375" bestFit="1" customWidth="1"/>
@@ -913,7 +992,7 @@
         <v>17</v>
       </c>
       <c r="E1" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="F1" t="s">
         <v>13</v>
@@ -931,13 +1010,13 @@
         <v>22</v>
       </c>
       <c r="K1" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="L1" t="s">
         <v>19</v>
       </c>
       <c r="M1" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -948,10 +1027,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="E2">
         <v>30</v>
@@ -989,10 +1068,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="E3">
         <v>11</v>
@@ -1030,10 +1109,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
+        <v>74</v>
       </c>
       <c r="E4">
         <v>48</v>
@@ -1142,7 +1221,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S3" sqref="S3"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1160,7 +1239,7 @@
         <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1171,7 +1250,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1182,7 +1261,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1193,7 +1272,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -1204,7 +1283,7 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -1215,7 +1294,7 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -1226,7 +1305,7 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -1237,7 +1316,7 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -1248,7 +1327,7 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -1259,7 +1338,7 @@
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1271,10 +1350,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{587ECBB5-A40B-459B-A765-E9FD0D7D4D73}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E18"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1282,7 +1361,7 @@
     <col min="1" max="1" width="11.125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.25" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="62.375" customWidth="1"/>
+    <col min="4" max="4" width="74.75" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="72.625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="40.625" customWidth="1"/>
   </cols>
@@ -1301,7 +1380,7 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -1315,10 +1394,10 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="E2" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -1332,10 +1411,10 @@
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E3" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1343,16 +1422,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="E4" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -1366,44 +1445,44 @@
         <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="E5" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="E6" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="D7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" t="s">
         <v>28</v>
-      </c>
-      <c r="E7" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -1414,13 +1493,13 @@
         <v>0</v>
       </c>
       <c r="C8" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="E8" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -1431,13 +1510,13 @@
         <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="E9" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -1445,16 +1524,16 @@
         <v>7</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="E10" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -1465,13 +1544,13 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="D11" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="E11" t="s">
-        <v>45</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -1482,13 +1561,13 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="D12" t="s">
-        <v>33</v>
+        <v>54</v>
       </c>
       <c r="E12" t="s">
-        <v>45</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -1499,13 +1578,13 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="D13" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="E13" t="s">
-        <v>45</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -1516,13 +1595,13 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="D14" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="E14" t="s">
-        <v>45</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -1533,13 +1612,13 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="D15" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="E15" t="s">
-        <v>45</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -1547,16 +1626,16 @@
         <v>7</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="D16" t="s">
-        <v>37</v>
+        <v>58</v>
       </c>
       <c r="E16" t="s">
-        <v>45</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -1567,13 +1646,13 @@
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="D17" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="E17" t="s">
-        <v>45</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -1584,13 +1663,64 @@
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="D18" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="E18" t="s">
-        <v>46</v>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" t="s">
+        <v>62</v>
+      </c>
+      <c r="E20" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" t="s">
+        <v>63</v>
+      </c>
+      <c r="E21" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1604,8 +1734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B24B819-66CE-4522-A8E9-8CAC3D8F6FB2}">
   <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1615,7 +1745,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -1626,7 +1756,7 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>60</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -1634,7 +1764,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1642,7 +1772,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -1650,7 +1780,7 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -1658,7 +1788,7 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -1666,97 +1796,132 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>66</v>
+        <v>40</v>
       </c>
       <c r="B8" t="s">
-        <v>67</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>66</v>
+        <v>40</v>
       </c>
       <c r="B9" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>66</v>
+        <v>40</v>
       </c>
       <c r="B10" t="s">
-        <v>69</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
+      <c r="A11" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B11" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
+      <c r="A12" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B12" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
+      <c r="A13" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B13" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
+      <c r="A14" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B14" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
+      <c r="A15" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B15" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="1"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="1"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B16" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B17" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">

</xml_diff>